<commit_message>
Add new feature and result files, update scripts
Added multiple new feature extraction and result files (XLSX and TXT) for syllables and vowels, including clean and selected features datasets. Updated .gitignore to exclude data and analysis directories. Modified and added scripts in src/ and src_analisi, and performed file renames and updates to maintain consistency in results and features directories.
</commit_message>
<xml_diff>
--- a/Features/Result presented/Old/vowels_clean.xlsx
+++ b/Features/Result presented/Old/vowels_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimos\Projects\VOC\Features\Result presented\Old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0C72B6-9168-41CE-8390-229EB31C788A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98310945-7B8D-4FB2-8558-73915E74D190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="374">
   <si>
     <t>subjid</t>
   </si>
@@ -1148,21 +1148,12 @@
   <si>
     <t>PZ115</t>
   </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Onset</t>
-  </si>
-  <si>
-    <t>Disease duration</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1184,11 +1175,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1246,16 +1232,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1590,7 +1573,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:JN101"/>
+  <dimension ref="A1:JK101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="IT1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="JI1" sqref="JI1:JK1048576"/>
@@ -1598,13 +1581,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="269" max="269" width="4.06640625" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="839" max="1027" width="9.1328125" customWidth="1"/>
+    <col min="836" max="1024" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2409,26 +2389,17 @@
       <c r="JH1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="JI1" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="JJ1" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="JK1" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="JL1" s="2" t="s">
+      <c r="JI1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="JM1" s="3" t="s">
+      <c r="JJ1" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="JN1" s="3" t="s">
+      <c r="JK1" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -3234,25 +3205,16 @@
         <v>-13.5399894714356</v>
       </c>
       <c r="JI2">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="JJ2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="JK2">
-        <v>8</v>
-      </c>
-      <c r="JL2">
-        <v>3</v>
-      </c>
-      <c r="JM2">
-        <v>2</v>
-      </c>
-      <c r="JN2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>275</v>
       </c>
@@ -4052,25 +4014,16 @@
         <v>-14.722516059875501</v>
       </c>
       <c r="JI3">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="JJ3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK3">
-        <v>23</v>
-      </c>
-      <c r="JL3">
-        <v>4</v>
-      </c>
-      <c r="JM3">
-        <v>3</v>
-      </c>
-      <c r="JN3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -4876,25 +4829,16 @@
         <v>-10.7034196853638</v>
       </c>
       <c r="JI4">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="JJ4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="JK4">
-        <v>55</v>
-      </c>
-      <c r="JL4">
-        <v>3</v>
-      </c>
-      <c r="JM4">
-        <v>3</v>
-      </c>
-      <c r="JN4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>277</v>
       </c>
@@ -5700,25 +5644,16 @@
         <v>-13.7495069503784</v>
       </c>
       <c r="JI5">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="JJ5">
+        <v>3</v>
+      </c>
+      <c r="JK5">
         <v>0</v>
       </c>
-      <c r="JK5">
-        <v>15</v>
-      </c>
-      <c r="JL5">
-        <v>3</v>
-      </c>
-      <c r="JM5">
-        <v>3</v>
-      </c>
-      <c r="JN5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>278</v>
       </c>
@@ -6524,25 +6459,16 @@
         <v>-13.897296905517599</v>
       </c>
       <c r="JI6">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="JJ6">
+        <v>2</v>
+      </c>
+      <c r="JK6">
         <v>1</v>
       </c>
-      <c r="JK6">
-        <v>11</v>
-      </c>
-      <c r="JL6">
-        <v>3</v>
-      </c>
-      <c r="JM6">
-        <v>2</v>
-      </c>
-      <c r="JN6">
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>279</v>
       </c>
@@ -7348,25 +7274,16 @@
         <v>-14.3713636398315</v>
       </c>
       <c r="JI7">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="JJ7">
+        <v>2</v>
+      </c>
+      <c r="JK7">
         <v>0</v>
       </c>
-      <c r="JK7">
-        <v>30</v>
-      </c>
-      <c r="JL7">
-        <v>2</v>
-      </c>
-      <c r="JM7">
-        <v>2</v>
-      </c>
-      <c r="JN7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>280</v>
       </c>
@@ -8172,25 +8089,16 @@
         <v>-13.4433403015137</v>
       </c>
       <c r="JI8">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="JJ8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK8">
-        <v>24</v>
-      </c>
-      <c r="JL8">
-        <v>2</v>
-      </c>
-      <c r="JM8">
-        <v>3</v>
-      </c>
-      <c r="JN8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>281</v>
       </c>
@@ -8996,25 +8904,16 @@
         <v>-14.150718688964799</v>
       </c>
       <c r="JI9">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="JJ9">
+        <v>3</v>
+      </c>
+      <c r="JK9">
         <v>0</v>
       </c>
-      <c r="JK9">
-        <v>29</v>
-      </c>
-      <c r="JL9">
-        <v>4</v>
-      </c>
-      <c r="JM9">
-        <v>3</v>
-      </c>
-      <c r="JN9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>282</v>
       </c>
@@ -9820,25 +9719,16 @@
         <v>-13.3691082000732</v>
       </c>
       <c r="JI10">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="JJ10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK10">
-        <v>27</v>
-      </c>
-      <c r="JL10">
         <v>2</v>
       </c>
-      <c r="JM10">
-        <v>2</v>
-      </c>
-      <c r="JN10">
-        <v>2</v>
-      </c>
     </row>
-    <row r="11" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>283</v>
       </c>
@@ -10644,25 +10534,16 @@
         <v>-13.7353630065918</v>
       </c>
       <c r="JI11">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="JJ11">
+        <v>4</v>
+      </c>
+      <c r="JK11">
         <v>0</v>
       </c>
-      <c r="JK11">
-        <v>15</v>
-      </c>
-      <c r="JL11">
-        <v>4</v>
-      </c>
-      <c r="JM11">
-        <v>4</v>
-      </c>
-      <c r="JN11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>284</v>
       </c>
@@ -11468,25 +11349,16 @@
         <v>-14.4646663665772</v>
       </c>
       <c r="JI12">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="JJ12">
+        <v>4</v>
+      </c>
+      <c r="JK12">
         <v>0</v>
       </c>
-      <c r="JK12">
-        <v>52</v>
-      </c>
-      <c r="JL12">
-        <v>4</v>
-      </c>
-      <c r="JM12">
-        <v>4</v>
-      </c>
-      <c r="JN12">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>285</v>
       </c>
@@ -12292,25 +12164,16 @@
         <v>-14.0951900482178</v>
       </c>
       <c r="JI13">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="JJ13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK13">
-        <v>18</v>
-      </c>
-      <c r="JL13">
         <v>3</v>
       </c>
-      <c r="JM13">
-        <v>3</v>
-      </c>
-      <c r="JN13">
-        <v>3</v>
-      </c>
     </row>
-    <row r="14" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>286</v>
       </c>
@@ -13113,25 +12976,16 @@
         <v>-12.245388984680201</v>
       </c>
       <c r="JI14">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="JJ14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK14">
-        <v>36</v>
-      </c>
-      <c r="JL14">
-        <v>4</v>
-      </c>
-      <c r="JM14">
-        <v>4</v>
-      </c>
-      <c r="JN14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>287</v>
       </c>
@@ -13937,25 +13791,16 @@
         <v>-13.8757629394531</v>
       </c>
       <c r="JI15">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="JJ15">
+        <v>4</v>
+      </c>
+      <c r="JK15">
         <v>0</v>
       </c>
-      <c r="JK15">
-        <v>12</v>
-      </c>
-      <c r="JL15">
-        <v>4</v>
-      </c>
-      <c r="JM15">
-        <v>4</v>
-      </c>
-      <c r="JN15">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>288</v>
       </c>
@@ -14761,25 +14606,16 @@
         <v>-13.0936012268066</v>
       </c>
       <c r="JI16">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="JJ16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="JK16">
         <v>2</v>
       </c>
-      <c r="JL16">
-        <v>3</v>
-      </c>
-      <c r="JM16">
-        <v>3</v>
-      </c>
-      <c r="JN16">
-        <v>2</v>
-      </c>
     </row>
-    <row r="17" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>289</v>
       </c>
@@ -15585,25 +15421,16 @@
         <v>-13.7425422668457</v>
       </c>
       <c r="JI17">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="JJ17">
+        <v>4</v>
+      </c>
+      <c r="JK17">
         <v>0</v>
       </c>
-      <c r="JK17">
-        <v>57</v>
-      </c>
-      <c r="JL17">
-        <v>4</v>
-      </c>
-      <c r="JM17">
-        <v>4</v>
-      </c>
-      <c r="JN17">
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>290</v>
       </c>
@@ -16409,25 +16236,16 @@
         <v>-13.1791934967041</v>
       </c>
       <c r="JI18">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="JJ18">
+        <v>4</v>
+      </c>
+      <c r="JK18">
         <v>0</v>
       </c>
-      <c r="JK18">
-        <v>7</v>
-      </c>
-      <c r="JL18">
-        <v>4</v>
-      </c>
-      <c r="JM18">
-        <v>4</v>
-      </c>
-      <c r="JN18">
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>291</v>
       </c>
@@ -17233,25 +17051,16 @@
         <v>-13.8971405029297</v>
       </c>
       <c r="JI19">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="JJ19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK19">
-        <v>10</v>
-      </c>
-      <c r="JL19">
-        <v>1</v>
-      </c>
-      <c r="JM19">
-        <v>2</v>
-      </c>
-      <c r="JN19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>292</v>
       </c>
@@ -18057,25 +17866,16 @@
         <v>-11.2950391769409</v>
       </c>
       <c r="JI20">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="JJ20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="JK20">
-        <v>12</v>
-      </c>
-      <c r="JL20">
-        <v>3</v>
-      </c>
-      <c r="JM20">
-        <v>3</v>
-      </c>
-      <c r="JN20">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>293</v>
       </c>
@@ -18881,25 +18681,16 @@
         <v>-13.769630432128899</v>
       </c>
       <c r="JI21">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="JJ21">
+        <v>4</v>
+      </c>
+      <c r="JK21">
         <v>0</v>
       </c>
-      <c r="JK21">
-        <v>15</v>
-      </c>
-      <c r="JL21">
-        <v>4</v>
-      </c>
-      <c r="JM21">
-        <v>4</v>
-      </c>
-      <c r="JN21">
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>294</v>
       </c>
@@ -19705,25 +19496,16 @@
         <v>-13.226848602294901</v>
       </c>
       <c r="JI22">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="JJ22">
+        <v>4</v>
+      </c>
+      <c r="JK22">
         <v>0</v>
       </c>
-      <c r="JK22">
-        <v>51</v>
-      </c>
-      <c r="JL22">
-        <v>4</v>
-      </c>
-      <c r="JM22">
-        <v>4</v>
-      </c>
-      <c r="JN22">
-        <v>0</v>
-      </c>
     </row>
-    <row r="23" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>295</v>
       </c>
@@ -20529,25 +20311,16 @@
         <v>-14.8260002136231</v>
       </c>
       <c r="JI23">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="JJ23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK23">
-        <v>49</v>
-      </c>
-      <c r="JL23">
         <v>3</v>
       </c>
-      <c r="JM23">
-        <v>3</v>
-      </c>
-      <c r="JN23">
-        <v>3</v>
-      </c>
     </row>
-    <row r="24" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>296</v>
       </c>
@@ -21353,25 +21126,16 @@
         <v>-12.9292039871216</v>
       </c>
       <c r="JI24">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="JJ24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK24">
-        <v>14</v>
-      </c>
-      <c r="JL24">
-        <v>4</v>
-      </c>
-      <c r="JM24">
-        <v>4</v>
-      </c>
-      <c r="JN24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>297</v>
       </c>
@@ -22177,25 +21941,16 @@
         <v>-14.7793588638306</v>
       </c>
       <c r="JI25">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="JJ25">
+        <v>4</v>
+      </c>
+      <c r="JK25">
         <v>0</v>
       </c>
-      <c r="JK25">
-        <v>38</v>
-      </c>
-      <c r="JL25">
-        <v>4</v>
-      </c>
-      <c r="JM25">
-        <v>4</v>
-      </c>
-      <c r="JN25">
-        <v>0</v>
-      </c>
     </row>
-    <row r="26" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>298</v>
       </c>
@@ -23001,25 +22756,16 @@
         <v>-13.2794437408447</v>
       </c>
       <c r="JI26">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="JJ26">
+        <v>4</v>
+      </c>
+      <c r="JK26">
         <v>0</v>
       </c>
-      <c r="JK26">
-        <v>8</v>
-      </c>
-      <c r="JL26">
-        <v>4</v>
-      </c>
-      <c r="JM26">
-        <v>4</v>
-      </c>
-      <c r="JN26">
-        <v>0</v>
-      </c>
     </row>
-    <row r="27" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>299</v>
       </c>
@@ -23825,25 +23571,16 @@
         <v>-13.8321037292481</v>
       </c>
       <c r="JI27">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="JJ27">
+        <v>3</v>
+      </c>
+      <c r="JK27">
         <v>0</v>
       </c>
-      <c r="JK27">
-        <v>106</v>
-      </c>
-      <c r="JL27">
-        <v>4</v>
-      </c>
-      <c r="JM27">
-        <v>3</v>
-      </c>
-      <c r="JN27">
-        <v>0</v>
-      </c>
     </row>
-    <row r="28" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>300</v>
       </c>
@@ -24649,25 +24386,16 @@
         <v>-13.3430089950562</v>
       </c>
       <c r="JI28">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="JJ28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK28">
-        <v>3</v>
-      </c>
-      <c r="JL28">
-        <v>4</v>
-      </c>
-      <c r="JM28">
-        <v>4</v>
-      </c>
-      <c r="JN28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>301</v>
       </c>
@@ -25473,25 +25201,16 @@
         <v>-14.5074415206909</v>
       </c>
       <c r="JI29">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="JJ29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="JK29">
-        <v>73</v>
-      </c>
-      <c r="JL29">
-        <v>4</v>
-      </c>
-      <c r="JM29">
-        <v>2</v>
-      </c>
-      <c r="JN29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>302</v>
       </c>
@@ -26297,25 +26016,16 @@
         <v>-10.9691486358643</v>
       </c>
       <c r="JI30">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="JJ30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK30">
-        <v>42</v>
-      </c>
-      <c r="JL30">
-        <v>3</v>
-      </c>
-      <c r="JM30">
-        <v>3</v>
-      </c>
-      <c r="JN30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>303</v>
       </c>
@@ -27121,25 +26831,16 @@
         <v>-14.257041931152299</v>
       </c>
       <c r="JI31">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="JJ31">
+        <v>4</v>
+      </c>
+      <c r="JK31">
         <v>0</v>
       </c>
-      <c r="JK31">
-        <v>52</v>
-      </c>
-      <c r="JL31">
-        <v>4</v>
-      </c>
-      <c r="JM31">
-        <v>4</v>
-      </c>
-      <c r="JN31">
-        <v>0</v>
-      </c>
     </row>
-    <row r="32" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>304</v>
       </c>
@@ -27945,25 +27646,16 @@
         <v>-12.6041316986084</v>
       </c>
       <c r="JI32">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="JJ32">
+        <v>3</v>
+      </c>
+      <c r="JK32">
         <v>0</v>
       </c>
-      <c r="JK32">
-        <v>68</v>
-      </c>
-      <c r="JL32">
-        <v>3</v>
-      </c>
-      <c r="JM32">
-        <v>3</v>
-      </c>
-      <c r="JN32">
-        <v>0</v>
-      </c>
     </row>
-    <row r="33" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>305</v>
       </c>
@@ -28769,25 +28461,16 @@
         <v>-14.6858978271484</v>
       </c>
       <c r="JI33">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="JJ33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK33">
-        <v>111</v>
-      </c>
-      <c r="JL33">
-        <v>4</v>
-      </c>
-      <c r="JM33">
-        <v>4</v>
-      </c>
-      <c r="JN33">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>306</v>
       </c>
@@ -29593,25 +29276,16 @@
         <v>-12.950594902038601</v>
       </c>
       <c r="JI34">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="JJ34">
+        <v>3</v>
+      </c>
+      <c r="JK34">
         <v>0</v>
       </c>
-      <c r="JK34">
-        <v>53</v>
-      </c>
-      <c r="JL34">
-        <v>4</v>
-      </c>
-      <c r="JM34">
-        <v>3</v>
-      </c>
-      <c r="JN34">
-        <v>0</v>
-      </c>
     </row>
-    <row r="35" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>307</v>
       </c>
@@ -30417,25 +30091,16 @@
         <v>-14.3288726806641</v>
       </c>
       <c r="JI35">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="JJ35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="JK35">
-        <v>2</v>
-      </c>
-      <c r="JL35">
-        <v>3</v>
-      </c>
-      <c r="JM35">
-        <v>4</v>
-      </c>
-      <c r="JN35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>308</v>
       </c>
@@ -31241,25 +30906,16 @@
         <v>-13.231280326843301</v>
       </c>
       <c r="JI36">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="JJ36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK36">
-        <v>27</v>
-      </c>
-      <c r="JL36">
-        <v>4</v>
-      </c>
-      <c r="JM36">
-        <v>4</v>
-      </c>
-      <c r="JN36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>309</v>
       </c>
@@ -32062,25 +31718,16 @@
         <v>-14.434452056884799</v>
       </c>
       <c r="JI37">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="JJ37">
+        <v>4</v>
+      </c>
+      <c r="JK37">
         <v>0</v>
       </c>
-      <c r="JK37">
-        <v>29</v>
-      </c>
-      <c r="JL37">
-        <v>4</v>
-      </c>
-      <c r="JM37">
-        <v>4</v>
-      </c>
-      <c r="JN37">
-        <v>0</v>
-      </c>
     </row>
-    <row r="38" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>310</v>
       </c>
@@ -32886,25 +32533,16 @@
         <v>-13.4394073486328</v>
       </c>
       <c r="JI38">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="JJ38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK38">
-        <v>59</v>
-      </c>
-      <c r="JL38">
-        <v>3</v>
-      </c>
-      <c r="JM38">
-        <v>2</v>
-      </c>
-      <c r="JN38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>311</v>
       </c>
@@ -33710,25 +33348,16 @@
         <v>-13.2242755889893</v>
       </c>
       <c r="JI39">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="JJ39">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK39">
-        <v>74</v>
-      </c>
-      <c r="JL39">
-        <v>4</v>
-      </c>
-      <c r="JM39">
-        <v>4</v>
-      </c>
-      <c r="JN39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>312</v>
       </c>
@@ -34534,25 +34163,16 @@
         <v>-13.9215698242188</v>
       </c>
       <c r="JI40">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="JJ40">
+        <v>3</v>
+      </c>
+      <c r="JK40">
         <v>0</v>
       </c>
-      <c r="JK40">
-        <v>8</v>
-      </c>
-      <c r="JL40">
-        <v>3</v>
-      </c>
-      <c r="JM40">
-        <v>3</v>
-      </c>
-      <c r="JN40">
-        <v>0</v>
-      </c>
     </row>
-    <row r="41" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>313</v>
       </c>
@@ -35358,25 +34978,16 @@
         <v>-12.500189781189</v>
       </c>
       <c r="JI41">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="JJ41">
+        <v>4</v>
+      </c>
+      <c r="JK41">
         <v>0</v>
       </c>
-      <c r="JK41">
-        <v>63</v>
-      </c>
-      <c r="JL41">
-        <v>4</v>
-      </c>
-      <c r="JM41">
-        <v>4</v>
-      </c>
-      <c r="JN41">
-        <v>0</v>
-      </c>
     </row>
-    <row r="42" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>314</v>
       </c>
@@ -36182,25 +35793,16 @@
         <v>-13.934718132019</v>
       </c>
       <c r="JI42">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="JJ42">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK42">
-        <v>49</v>
-      </c>
-      <c r="JL42">
-        <v>4</v>
-      </c>
-      <c r="JM42">
-        <v>4</v>
-      </c>
-      <c r="JN42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>315</v>
       </c>
@@ -37006,25 +36608,16 @@
         <v>-8.0640764236450195</v>
       </c>
       <c r="JI43">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="JJ43">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK43">
-        <v>9</v>
-      </c>
-      <c r="JL43">
-        <v>4</v>
-      </c>
-      <c r="JM43">
-        <v>4</v>
-      </c>
-      <c r="JN43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>316</v>
       </c>
@@ -37830,25 +37423,16 @@
         <v>-10.865893363952599</v>
       </c>
       <c r="JI44">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="JJ44">
+        <v>4</v>
+      </c>
+      <c r="JK44">
         <v>0</v>
       </c>
-      <c r="JK44">
-        <v>9</v>
-      </c>
-      <c r="JL44">
-        <v>4</v>
-      </c>
-      <c r="JM44">
-        <v>4</v>
-      </c>
-      <c r="JN44">
-        <v>0</v>
-      </c>
     </row>
-    <row r="45" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>317</v>
       </c>
@@ -38654,25 +38238,16 @@
         <v>-12.192430496215801</v>
       </c>
       <c r="JI45">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="JJ45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK45">
-        <v>8</v>
-      </c>
-      <c r="JL45">
-        <v>1</v>
-      </c>
-      <c r="JM45">
-        <v>2</v>
-      </c>
-      <c r="JN45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>318</v>
       </c>
@@ -39478,25 +39053,16 @@
         <v>-15.857781410217299</v>
       </c>
       <c r="JI46">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="JJ46">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK46">
-        <v>9</v>
-      </c>
-      <c r="JL46">
-        <v>4</v>
-      </c>
-      <c r="JM46">
-        <v>4</v>
-      </c>
-      <c r="JN46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>319</v>
       </c>
@@ -40302,25 +39868,16 @@
         <v>-10.5153961181641</v>
       </c>
       <c r="JI47">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="JJ47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK47">
-        <v>10</v>
-      </c>
-      <c r="JL47">
-        <v>4</v>
-      </c>
-      <c r="JM47">
-        <v>4</v>
-      </c>
-      <c r="JN47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>320</v>
       </c>
@@ -41126,25 +40683,16 @@
         <v>-12.935590744018601</v>
       </c>
       <c r="JI48">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="JJ48">
+        <v>4</v>
+      </c>
+      <c r="JK48">
         <v>0</v>
       </c>
-      <c r="JK48">
-        <v>52</v>
-      </c>
-      <c r="JL48">
-        <v>4</v>
-      </c>
-      <c r="JM48">
-        <v>4</v>
-      </c>
-      <c r="JN48">
-        <v>0</v>
-      </c>
     </row>
-    <row r="49" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>321</v>
       </c>
@@ -41950,25 +41498,16 @@
         <v>-13.3402366638184</v>
       </c>
       <c r="JI49">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="JJ49">
+        <v>3</v>
+      </c>
+      <c r="JK49">
         <v>0</v>
       </c>
-      <c r="JK49">
-        <v>151</v>
-      </c>
-      <c r="JL49">
-        <v>4</v>
-      </c>
-      <c r="JM49">
-        <v>3</v>
-      </c>
-      <c r="JN49">
-        <v>0</v>
-      </c>
     </row>
-    <row r="50" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>322</v>
       </c>
@@ -42774,25 +42313,16 @@
         <v>-12.007626533508301</v>
       </c>
       <c r="JI50">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="JJ50">
+        <v>4</v>
+      </c>
+      <c r="JK50">
         <v>0</v>
       </c>
-      <c r="JK50">
-        <v>13</v>
-      </c>
-      <c r="JL50">
-        <v>3</v>
-      </c>
-      <c r="JM50">
-        <v>4</v>
-      </c>
-      <c r="JN50">
-        <v>0</v>
-      </c>
     </row>
-    <row r="51" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>323</v>
       </c>
@@ -43598,25 +43128,16 @@
         <v>-12.4585771560669</v>
       </c>
       <c r="JI51">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="JJ51">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK51">
-        <v>15</v>
-      </c>
-      <c r="JL51">
-        <v>4</v>
-      </c>
-      <c r="JM51">
-        <v>4</v>
-      </c>
-      <c r="JN51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>324</v>
       </c>
@@ -44422,25 +43943,16 @@
         <v>-14.333133697509799</v>
       </c>
       <c r="JI52">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="JJ52">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK52">
-        <v>25</v>
-      </c>
-      <c r="JL52">
-        <v>3</v>
-      </c>
-      <c r="JM52">
-        <v>4</v>
-      </c>
-      <c r="JN52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>325</v>
       </c>
@@ -45246,25 +44758,16 @@
         <v>-13.0462398529053</v>
       </c>
       <c r="JI53">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="JJ53">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK53">
-        <v>5</v>
-      </c>
-      <c r="JL53">
-        <v>4</v>
-      </c>
-      <c r="JM53">
-        <v>4</v>
-      </c>
-      <c r="JN53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>326</v>
       </c>
@@ -46070,25 +45573,16 @@
         <v>-14.6630096435547</v>
       </c>
       <c r="JI54">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="JJ54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK54">
-        <v>5</v>
-      </c>
-      <c r="JL54">
-        <v>3</v>
-      </c>
-      <c r="JM54">
-        <v>4</v>
-      </c>
-      <c r="JN54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>327</v>
       </c>
@@ -46894,25 +46388,16 @@
         <v>-15.156675338745099</v>
       </c>
       <c r="JI55">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="JJ55">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK55">
-        <v>24</v>
-      </c>
-      <c r="JL55">
-        <v>4</v>
-      </c>
-      <c r="JM55">
-        <v>4</v>
-      </c>
-      <c r="JN55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>328</v>
       </c>
@@ -47718,25 +47203,16 @@
         <v>-13.2748584747315</v>
       </c>
       <c r="JI56">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="JJ56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK56">
-        <v>33</v>
-      </c>
-      <c r="JL56">
-        <v>4</v>
-      </c>
-      <c r="JM56">
-        <v>4</v>
-      </c>
-      <c r="JN56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>329</v>
       </c>
@@ -48539,25 +48015,16 @@
         <v>-14.3477878570557</v>
       </c>
       <c r="JI57">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="JJ57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK57">
-        <v>3</v>
-      </c>
-      <c r="JL57">
-        <v>1</v>
-      </c>
-      <c r="JM57">
-        <v>2</v>
-      </c>
-      <c r="JN57">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>330</v>
       </c>
@@ -49363,25 +48830,16 @@
         <v>-14.22864818573</v>
       </c>
       <c r="JI58">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="JJ58">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK58">
-        <v>63</v>
-      </c>
-      <c r="JL58">
-        <v>3</v>
-      </c>
-      <c r="JM58">
-        <v>3</v>
-      </c>
-      <c r="JN58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>331</v>
       </c>
@@ -50187,25 +49645,16 @@
         <v>-13.43385887146</v>
       </c>
       <c r="JI59">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="JJ59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK59">
-        <v>7</v>
-      </c>
-      <c r="JL59">
-        <v>3</v>
-      </c>
-      <c r="JM59">
-        <v>2</v>
-      </c>
-      <c r="JN59">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>332</v>
       </c>
@@ -51011,25 +50460,16 @@
         <v>-11.930301666259799</v>
       </c>
       <c r="JI60">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="JJ60">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK60">
-        <v>14</v>
-      </c>
-      <c r="JL60">
-        <v>4</v>
-      </c>
-      <c r="JM60">
-        <v>4</v>
-      </c>
-      <c r="JN60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>333</v>
       </c>
@@ -51835,25 +51275,16 @@
         <v>-13.5602922439575</v>
       </c>
       <c r="JI61">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="JJ61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK61">
-        <v>20</v>
-      </c>
-      <c r="JL61">
-        <v>3</v>
-      </c>
-      <c r="JM61">
-        <v>4</v>
-      </c>
-      <c r="JN61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>334</v>
       </c>
@@ -52659,25 +52090,16 @@
         <v>-10.1452169418335</v>
       </c>
       <c r="JI62">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="JJ62">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK62">
-        <v>21</v>
-      </c>
-      <c r="JL62">
         <v>3</v>
       </c>
-      <c r="JM62">
-        <v>3</v>
-      </c>
-      <c r="JN62">
-        <v>3</v>
-      </c>
     </row>
-    <row r="63" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>335</v>
       </c>
@@ -53483,25 +52905,16 @@
         <v>-14.5186719894409</v>
       </c>
       <c r="JI63">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="JJ63">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK63">
-        <v>14</v>
-      </c>
-      <c r="JL63">
-        <v>3</v>
-      </c>
-      <c r="JM63">
-        <v>4</v>
-      </c>
-      <c r="JN63">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>336</v>
       </c>
@@ -54307,25 +53720,16 @@
         <v>-13.9238195419312</v>
       </c>
       <c r="JI64">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="JJ64">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK64">
-        <v>9</v>
-      </c>
-      <c r="JL64">
-        <v>3</v>
-      </c>
-      <c r="JM64">
-        <v>3</v>
-      </c>
-      <c r="JN64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>337</v>
       </c>
@@ -55131,25 +54535,16 @@
         <v>-13.635422706604</v>
       </c>
       <c r="JI65">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="JJ65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="JK65">
-        <v>93</v>
-      </c>
-      <c r="JL65">
-        <v>2</v>
-      </c>
-      <c r="JM65">
-        <v>2</v>
-      </c>
-      <c r="JN65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>338</v>
       </c>
@@ -55955,25 +55350,16 @@
         <v>-13.3666276931763</v>
       </c>
       <c r="JI66">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="JJ66">
+        <v>4</v>
+      </c>
+      <c r="JK66">
         <v>0</v>
       </c>
-      <c r="JK66">
-        <v>37</v>
-      </c>
-      <c r="JL66">
-        <v>3</v>
-      </c>
-      <c r="JM66">
-        <v>4</v>
-      </c>
-      <c r="JN66">
-        <v>0</v>
-      </c>
     </row>
-    <row r="67" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>339</v>
       </c>
@@ -56779,25 +56165,16 @@
         <v>-12.620399475097701</v>
       </c>
       <c r="JI67">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="JJ67">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="JK67">
-        <v>19</v>
-      </c>
-      <c r="JL67">
-        <v>1</v>
-      </c>
-      <c r="JM67">
-        <v>4</v>
-      </c>
-      <c r="JN67">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>340</v>
       </c>
@@ -57603,25 +56980,16 @@
         <v>-14.3978481292725</v>
       </c>
       <c r="JI68">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="JJ68">
+        <v>4</v>
+      </c>
+      <c r="JK68">
         <v>0</v>
       </c>
-      <c r="JK68">
-        <v>27</v>
-      </c>
-      <c r="JL68">
-        <v>4</v>
-      </c>
-      <c r="JM68">
-        <v>4</v>
-      </c>
-      <c r="JN68">
-        <v>0</v>
-      </c>
     </row>
-    <row r="69" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>341</v>
       </c>
@@ -58421,25 +57789,16 @@
         <v>-9.4244775772094709</v>
       </c>
       <c r="JI69">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="JJ69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK69">
         <v>4</v>
       </c>
-      <c r="JL69">
-        <v>2</v>
-      </c>
-      <c r="JM69">
-        <v>2</v>
-      </c>
-      <c r="JN69">
-        <v>4</v>
-      </c>
     </row>
-    <row r="70" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>342</v>
       </c>
@@ -59245,25 +58604,16 @@
         <v>-14.112225532531699</v>
       </c>
       <c r="JI70">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="JJ70">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK70">
-        <v>39</v>
-      </c>
-      <c r="JL70">
-        <v>4</v>
-      </c>
-      <c r="JM70">
-        <v>4</v>
-      </c>
-      <c r="JN70">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>343</v>
       </c>
@@ -60066,25 +59416,16 @@
         <v>-14.57834815979</v>
       </c>
       <c r="JI71">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="JJ71">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK71">
-        <v>22</v>
-      </c>
-      <c r="JL71">
-        <v>4</v>
-      </c>
-      <c r="JM71">
-        <v>4</v>
-      </c>
-      <c r="JN71">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>344</v>
       </c>
@@ -60890,25 +60231,16 @@
         <v>-14.4167928695679</v>
       </c>
       <c r="JI72">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="JJ72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="JK72">
-        <v>4</v>
-      </c>
-      <c r="JL72">
-        <v>3</v>
-      </c>
-      <c r="JM72">
-        <v>2</v>
-      </c>
-      <c r="JN72">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>345</v>
       </c>
@@ -61711,25 +61043,16 @@
         <v>-12.979500770568899</v>
       </c>
       <c r="JI73">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="JJ73">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK73">
-        <v>8</v>
-      </c>
-      <c r="JL73">
-        <v>4</v>
-      </c>
-      <c r="JM73">
-        <v>4</v>
-      </c>
-      <c r="JN73">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>346</v>
       </c>
@@ -62532,25 +61855,16 @@
         <v>-13.328693389892599</v>
       </c>
       <c r="JI74">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="JJ74">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK74">
-        <v>26</v>
-      </c>
-      <c r="JL74">
-        <v>4</v>
-      </c>
-      <c r="JM74">
-        <v>3</v>
-      </c>
-      <c r="JN74">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>347</v>
       </c>
@@ -63356,25 +62670,16 @@
         <v>-14.615642547607401</v>
       </c>
       <c r="JI75">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="JJ75">
+        <v>4</v>
+      </c>
+      <c r="JK75">
         <v>0</v>
       </c>
-      <c r="JK75">
-        <v>3</v>
-      </c>
-      <c r="JL75">
-        <v>4</v>
-      </c>
-      <c r="JM75">
-        <v>4</v>
-      </c>
-      <c r="JN75">
-        <v>0</v>
-      </c>
     </row>
-    <row r="76" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>348</v>
       </c>
@@ -64180,25 +63485,16 @@
         <v>-14.9713134765625</v>
       </c>
       <c r="JI76">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="JJ76">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK76">
-        <v>17</v>
-      </c>
-      <c r="JL76">
-        <v>4</v>
-      </c>
-      <c r="JM76">
-        <v>3</v>
-      </c>
-      <c r="JN76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>349</v>
       </c>
@@ -65004,25 +64300,16 @@
         <v>-14.955930709838899</v>
       </c>
       <c r="JI77">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="JJ77">
+        <v>3</v>
+      </c>
+      <c r="JK77">
         <v>1</v>
       </c>
-      <c r="JK77">
-        <v>5</v>
-      </c>
-      <c r="JL77">
-        <v>2</v>
-      </c>
-      <c r="JM77">
-        <v>3</v>
-      </c>
-      <c r="JN77">
-        <v>1</v>
-      </c>
     </row>
-    <row r="78" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>350</v>
       </c>
@@ -65825,25 +65112,16 @@
         <v>-14.2268056869507</v>
       </c>
       <c r="JI78">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="JJ78">
+        <v>4</v>
+      </c>
+      <c r="JK78">
         <v>0</v>
       </c>
-      <c r="JK78">
-        <v>43</v>
-      </c>
-      <c r="JL78">
-        <v>4</v>
-      </c>
-      <c r="JM78">
-        <v>4</v>
-      </c>
-      <c r="JN78">
-        <v>0</v>
-      </c>
     </row>
-    <row r="79" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>351</v>
       </c>
@@ -66649,25 +65927,16 @@
         <v>-14.3341569900513</v>
       </c>
       <c r="JI79">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="JJ79">
         <v>1</v>
       </c>
       <c r="JK79">
-        <v>6</v>
-      </c>
-      <c r="JL79">
-        <v>2</v>
-      </c>
-      <c r="JM79">
-        <v>1</v>
-      </c>
-      <c r="JN79">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>352</v>
       </c>
@@ -67473,25 +66742,16 @@
         <v>-13.4962377548218</v>
       </c>
       <c r="JI80">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="JJ80">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK80">
-        <v>34</v>
-      </c>
-      <c r="JL80">
-        <v>4</v>
-      </c>
-      <c r="JM80">
-        <v>4</v>
-      </c>
-      <c r="JN80">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>353</v>
       </c>
@@ -68297,25 +67557,16 @@
         <v>-13.0716753005981</v>
       </c>
       <c r="JI81">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="JJ81">
+        <v>4</v>
+      </c>
+      <c r="JK81">
         <v>0</v>
       </c>
-      <c r="JK81">
-        <v>13</v>
-      </c>
-      <c r="JL81">
-        <v>4</v>
-      </c>
-      <c r="JM81">
-        <v>4</v>
-      </c>
-      <c r="JN81">
-        <v>0</v>
-      </c>
     </row>
-    <row r="82" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>354</v>
       </c>
@@ -69118,25 +68369,16 @@
         <v>-14.853218078613301</v>
       </c>
       <c r="JI82">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="JJ82">
+        <v>4</v>
+      </c>
+      <c r="JK82">
         <v>0</v>
       </c>
-      <c r="JK82">
-        <v>9</v>
-      </c>
-      <c r="JL82">
-        <v>4</v>
-      </c>
-      <c r="JM82">
-        <v>4</v>
-      </c>
-      <c r="JN82">
-        <v>0</v>
-      </c>
     </row>
-    <row r="83" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>355</v>
       </c>
@@ -69942,25 +69184,16 @@
         <v>-13.9161376953125</v>
       </c>
       <c r="JI83">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="JJ83">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK83">
-        <v>15</v>
-      </c>
-      <c r="JL83">
-        <v>3</v>
-      </c>
-      <c r="JM83">
-        <v>4</v>
-      </c>
-      <c r="JN83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>356</v>
       </c>
@@ -70766,25 +69999,16 @@
         <v>-13.5360679626465</v>
       </c>
       <c r="JI84">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="JJ84">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK84">
-        <v>4</v>
-      </c>
-      <c r="JL84">
-        <v>4</v>
-      </c>
-      <c r="JM84">
-        <v>4</v>
-      </c>
-      <c r="JN84">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>357</v>
       </c>
@@ -71587,25 +70811,16 @@
         <v>-9.1071691513061506</v>
       </c>
       <c r="JI85">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="JJ85">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="JK85">
-        <v>6</v>
-      </c>
-      <c r="JL85">
-        <v>2</v>
-      </c>
-      <c r="JM85">
-        <v>2</v>
-      </c>
-      <c r="JN85">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>358</v>
       </c>
@@ -72411,25 +71626,16 @@
         <v>-12.723997116088899</v>
       </c>
       <c r="JI86">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="JJ86">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK86">
-        <v>19</v>
-      </c>
-      <c r="JL86">
-        <v>4</v>
-      </c>
-      <c r="JM86">
-        <v>4</v>
-      </c>
-      <c r="JN86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>359</v>
       </c>
@@ -73235,25 +72441,16 @@
         <v>-14.5007762908935</v>
       </c>
       <c r="JI87">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="JJ87">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK87">
-        <v>16</v>
-      </c>
-      <c r="JL87">
-        <v>4</v>
-      </c>
-      <c r="JM87">
-        <v>4</v>
-      </c>
-      <c r="JN87">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>360</v>
       </c>
@@ -74056,25 +73253,16 @@
         <v>-14.535496711731</v>
       </c>
       <c r="JI88">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="JJ88">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK88">
-        <v>9</v>
-      </c>
-      <c r="JL88">
         <v>3</v>
       </c>
-      <c r="JM88">
-        <v>4</v>
-      </c>
-      <c r="JN88">
-        <v>3</v>
-      </c>
     </row>
-    <row r="89" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>361</v>
       </c>
@@ -74880,25 +74068,16 @@
         <v>-14.658084869384799</v>
       </c>
       <c r="JI89">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="JJ89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="JK89">
-        <v>114</v>
-      </c>
-      <c r="JL89">
         <v>2</v>
       </c>
-      <c r="JM89">
-        <v>2</v>
-      </c>
-      <c r="JN89">
-        <v>2</v>
-      </c>
     </row>
-    <row r="90" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>362</v>
       </c>
@@ -75704,25 +74883,16 @@
         <v>-13.550676345825201</v>
       </c>
       <c r="JI90">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="JJ90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="JK90">
-        <v>7</v>
-      </c>
-      <c r="JL90">
-        <v>2</v>
-      </c>
-      <c r="JM90">
-        <v>3</v>
-      </c>
-      <c r="JN90">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>363</v>
       </c>
@@ -76525,25 +75695,16 @@
         <v>-12.3569192886353</v>
       </c>
       <c r="JI91">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="JJ91">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK91">
-        <v>120</v>
-      </c>
-      <c r="JL91">
-        <v>3</v>
-      </c>
-      <c r="JM91">
-        <v>4</v>
-      </c>
-      <c r="JN91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>364</v>
       </c>
@@ -77349,25 +76510,16 @@
         <v>-14.645402908325201</v>
       </c>
       <c r="JI92">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="JJ92">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK92">
-        <v>3</v>
-      </c>
-      <c r="JL92">
-        <v>3</v>
-      </c>
-      <c r="JM92">
-        <v>3</v>
-      </c>
-      <c r="JN92">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>365</v>
       </c>
@@ -78173,25 +77325,16 @@
         <v>-13.482383728027299</v>
       </c>
       <c r="JI93">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="JJ93">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="JK93">
-        <v>2</v>
-      </c>
-      <c r="JL93">
         <v>3</v>
       </c>
-      <c r="JM93">
-        <v>3</v>
-      </c>
-      <c r="JN93">
-        <v>3</v>
-      </c>
     </row>
-    <row r="94" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>366</v>
       </c>
@@ -78997,25 +78140,16 @@
         <v>-12.6955261230469</v>
       </c>
       <c r="JI94">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="JJ94">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="JK94">
-        <v>10</v>
-      </c>
-      <c r="JL94">
-        <v>2</v>
-      </c>
-      <c r="JM94">
         <v>3</v>
       </c>
-      <c r="JN94">
-        <v>3</v>
-      </c>
     </row>
-    <row r="95" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>367</v>
       </c>
@@ -79821,25 +78955,16 @@
         <v>-13.7847909927368</v>
       </c>
       <c r="JI95">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="JJ95">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK95">
-        <v>6</v>
-      </c>
-      <c r="JL95">
-        <v>4</v>
-      </c>
-      <c r="JM95">
-        <v>4</v>
-      </c>
-      <c r="JN95">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>368</v>
       </c>
@@ -80645,25 +79770,16 @@
         <v>-13.8451690673828</v>
       </c>
       <c r="JI96">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="JJ96">
+        <v>4</v>
+      </c>
+      <c r="JK96">
         <v>0</v>
       </c>
-      <c r="JK96">
-        <v>17</v>
-      </c>
-      <c r="JL96">
-        <v>4</v>
-      </c>
-      <c r="JM96">
-        <v>4</v>
-      </c>
-      <c r="JN96">
-        <v>0</v>
-      </c>
     </row>
-    <row r="97" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>369</v>
       </c>
@@ -81469,25 +80585,16 @@
         <v>-12.087886810302701</v>
       </c>
       <c r="JI97">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="JJ97">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="JK97">
-        <v>37</v>
-      </c>
-      <c r="JL97">
-        <v>3</v>
-      </c>
-      <c r="JM97">
-        <v>3</v>
-      </c>
-      <c r="JN97">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>370</v>
       </c>
@@ -82293,25 +81400,16 @@
         <v>-13.4410076141357</v>
       </c>
       <c r="JI98">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="JJ98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="JK98">
-        <v>3</v>
-      </c>
-      <c r="JL98">
         <v>2</v>
       </c>
-      <c r="JM98">
-        <v>3</v>
-      </c>
-      <c r="JN98">
-        <v>2</v>
-      </c>
     </row>
-    <row r="99" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>371</v>
       </c>
@@ -83117,25 +82215,16 @@
         <v>-12.6630296707153</v>
       </c>
       <c r="JI99">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="JJ99">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="JK99">
-        <v>8</v>
-      </c>
-      <c r="JL99">
-        <v>2</v>
-      </c>
-      <c r="JM99">
-        <v>2</v>
-      </c>
-      <c r="JN99">
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>372</v>
       </c>
@@ -83941,25 +83030,16 @@
         <v>-11.347984313964799</v>
       </c>
       <c r="JI100">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="JJ100">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK100">
-        <v>8</v>
-      </c>
-      <c r="JL100">
-        <v>3</v>
-      </c>
-      <c r="JM100">
-        <v>4</v>
-      </c>
-      <c r="JN100">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:274" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:271" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>373</v>
       </c>
@@ -84765,21 +83845,12 @@
         <v>-13.6087436676025</v>
       </c>
       <c r="JI101">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="JJ101">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="JK101">
-        <v>6</v>
-      </c>
-      <c r="JL101">
-        <v>4</v>
-      </c>
-      <c r="JM101">
-        <v>4</v>
-      </c>
-      <c r="JN101">
         <v>3</v>
       </c>
     </row>

</xml_diff>